<commit_message>
Updated config file 3
</commit_message>
<xml_diff>
--- a/Resources/Configuration3.xlsx
+++ b/Resources/Configuration3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MugunthRaman\git\EagleAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449759EC-5633-4CED-8052-C8BF0D6C929E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3979F1F9-B339-4D69-A161-1D00E6204862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3883F32-F6B7-4344-89C2-CDCBDBE1FA77}"/>
   </bookViews>
@@ -798,9 +798,6 @@
     <t>&lt;Comparison Name to be selected&gt;,  &lt;entity to be selected&gt;, &lt;Case set Name to be added&gt;, &lt;search text for creating additional case set&gt;</t>
   </si>
   <si>
-    <t>Comparison Control and Case 1, Disease, Case Set2,soy</t>
-  </si>
-  <si>
     <t>SearchInComparisonExpand</t>
   </si>
   <si>
@@ -1137,7 +1134,10 @@
     <t>ComAddfromFile 1,Control Card, Disease,kera,Disease, C:\Users\eagleqateam\Documents\GitHub\SeleniumAutomation\Resources\Q4 - Upload file - 1 (2).xlsx, Q4 - Upload file - 1 (2).xlsx</t>
   </si>
   <si>
-    <t>GridSet, Disease, Kera, 10, EFO ID, Datasource Name</t>
+    <t>GridSet, Disease, Kera, 10, Definition, Identifier</t>
+  </si>
+  <si>
+    <t>Comparison Control and Case 1_222840, Disease, Case Set2,sor</t>
   </si>
 </sst>
 </file>
@@ -1550,75 +1550,21 @@
   <dxfs count="6">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1634,14 +1580,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B2293B69-6BEF-4876-8041-4E581FDF60A3}" name="Table22" displayName="Table22" ref="A1:E80" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E80" xr:uid="{B2293B69-6BEF-4876-8041-4E581FDF60A3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9F58C19D-99E7-4933-ADBF-D8A1FC7A4A8F}" name="Table2" displayName="Table2" ref="A1:E80" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E80" xr:uid="{9F58C19D-99E7-4933-ADBF-D8A1FC7A4A8F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{278089CD-41AD-4D0D-A37B-C3F0D49F8E08}" name="Test Case#" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{2B1CEA1A-9C99-4538-BF02-BDB38E61E3CE}" name="FunctionName" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{C6027479-92EE-49EA-B476-5EA7BCF3796C}" name="Description" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{8C627C27-DA49-4E96-9923-45AC6780212C}" name="Parameters" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{75315E8A-E375-4AC6-B082-FB25BA079233}" name="Test Data" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{E4EE8482-C9A5-4BE2-A04A-30789F6C4A9B}" name="Test Case#" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{6C42973B-7CD5-4DF3-A4E4-2D87D248B024}" name="FunctionName" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{079A4983-2A8D-4907-B9B0-A6044100813F}" name="Description" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{0BAF0785-F083-4DA1-ADB8-119AD848D105}" name="Parameters" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{63437997-297B-4FEB-8AB9-1175957F5FC1}" name="Test Data" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1946,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6CDC57-9314-4DDE-912B-780BF34D9001}">
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C59" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2162,7 +2108,7 @@
         <v>66</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G11" s="32"/>
       <c r="H11" s="10"/>
@@ -2257,7 +2203,7 @@
         <v>90</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G16" s="32"/>
       <c r="H16" s="10"/>
@@ -2299,7 +2245,7 @@
       </c>
       <c r="G18" s="32"/>
       <c r="H18" s="28" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2316,7 +2262,7 @@
         <v>103</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G19" s="32"/>
       <c r="H19" s="10"/>
@@ -2434,7 +2380,7 @@
       </c>
       <c r="G25" s="32"/>
       <c r="H25" s="28" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2455,7 +2401,7 @@
       </c>
       <c r="G26" s="33"/>
       <c r="H26" s="28" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2531,7 +2477,7 @@
         <v>149</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G30" s="34"/>
       <c r="H30" s="10"/>
@@ -2664,7 +2610,7 @@
         <v>182</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G37" s="34"/>
       <c r="H37" s="10"/>
@@ -2801,7 +2747,7 @@
       </c>
       <c r="G44" s="34"/>
       <c r="H44" s="28" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2841,7 +2787,7 @@
       </c>
       <c r="G46" s="34"/>
       <c r="H46" s="28" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2862,7 +2808,7 @@
       </c>
       <c r="G47" s="35"/>
       <c r="H47" s="28" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2919,7 +2865,7 @@
         <v>240</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G50" s="34"/>
       <c r="H50" s="10"/>
@@ -2976,349 +2922,349 @@
         <v>253</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>254</v>
+        <v>367</v>
       </c>
       <c r="G53" s="34"/>
       <c r="H53" s="10"/>
     </row>
     <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="E54" s="6" t="s">
         <v>258</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>259</v>
       </c>
       <c r="G54" s="34"/>
       <c r="H54" s="10"/>
     </row>
     <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="E55" s="6" t="s">
         <v>263</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>264</v>
       </c>
       <c r="G55" s="34"/>
       <c r="H55" s="10"/>
     </row>
     <row r="56" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="D56" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E56" s="6" t="s">
         <v>267</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>268</v>
       </c>
       <c r="G56" s="34"/>
       <c r="H56" s="10"/>
     </row>
     <row r="57" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="E57" s="6" t="s">
         <v>272</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>273</v>
       </c>
       <c r="G57" s="34"/>
       <c r="H57" s="10"/>
     </row>
     <row r="58" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="E58" s="6" t="s">
         <v>277</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>278</v>
       </c>
       <c r="G58" s="34"/>
       <c r="H58" s="10"/>
     </row>
     <row r="59" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="E59" s="6" t="s">
         <v>282</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>283</v>
       </c>
       <c r="G59" s="34"/>
       <c r="H59" s="10"/>
     </row>
     <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>286</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>90</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G60" s="34"/>
       <c r="H60" s="10"/>
     </row>
     <row r="61" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="E61" s="6" t="s">
         <v>290</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>291</v>
       </c>
       <c r="G61" s="34"/>
       <c r="H61" s="10"/>
     </row>
     <row r="62" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="D62" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E62" s="6" t="s">
         <v>294</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>295</v>
       </c>
       <c r="G62" s="34"/>
       <c r="H62" s="10"/>
     </row>
     <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="E63" s="6" t="s">
         <v>299</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>300</v>
       </c>
       <c r="G63" s="34"/>
       <c r="H63" s="10"/>
     </row>
     <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="E64" s="6" t="s">
         <v>304</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>305</v>
       </c>
       <c r="G64" s="34"/>
       <c r="H64" s="10"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="D65" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="E65" s="6" t="s">
         <v>309</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>310</v>
       </c>
       <c r="G65" s="34"/>
       <c r="H65" s="10"/>
     </row>
     <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="E66" s="6" t="s">
         <v>314</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>315</v>
       </c>
       <c r="G66" s="34"/>
       <c r="H66" s="10"/>
     </row>
     <row r="67" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="E67" s="6" t="s">
         <v>319</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>320</v>
       </c>
       <c r="G67" s="34"/>
       <c r="H67" s="10"/>
     </row>
     <row r="68" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="D68" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="E68" s="6" t="s">
         <v>324</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>325</v>
       </c>
       <c r="G68" s="34"/>
       <c r="H68" s="10"/>
     </row>
     <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="D69" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="E69" s="6" t="s">
         <v>329</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>330</v>
       </c>
       <c r="G69" s="34"/>
       <c r="H69" s="10"/>
     </row>
     <row r="70" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>332</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>333</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>225</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G70" s="34"/>
       <c r="H70" s="10"/>
     </row>
     <row r="71" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="C71" s="23" t="s">
         <v>336</v>
-      </c>
-      <c r="C71" s="23" t="s">
-        <v>337</v>
       </c>
       <c r="D71" s="23" t="s">
         <v>230</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G71" s="34"/>
       <c r="H71" s="10"/>
@@ -3342,93 +3288,93 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="E73" s="6" t="s">
         <v>340</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>341</v>
       </c>
       <c r="G73" s="30"/>
       <c r="H73" s="10"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="E74" s="6" t="s">
         <v>343</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>344</v>
       </c>
       <c r="G74" s="30"/>
       <c r="H74" s="10"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="E75" s="6" t="s">
         <v>346</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>347</v>
       </c>
       <c r="G75" s="30"/>
       <c r="H75" s="10"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="E76" s="6" t="s">
         <v>349</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>350</v>
       </c>
       <c r="G76" s="30"/>
       <c r="H76" s="10"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="E77" s="6" t="s">
         <v>352</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>353</v>
       </c>
       <c r="G77" s="30"/>
       <c r="H77" s="10"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="E78" s="6" t="s">
         <v>355</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>356</v>
       </c>
       <c r="G78" s="30"/>
       <c r="H78" s="10"/>
     </row>
     <row r="79" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="26" t="s">
+        <v>356</v>
+      </c>
+      <c r="B79" s="23" t="s">
         <v>357</v>
-      </c>
-      <c r="B79" s="23" t="s">
-        <v>358</v>
       </c>
       <c r="C79" s="23"/>
       <c r="D79" s="23"/>
       <c r="E79" s="25" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G79" s="37"/>
       <c r="H79" s="10"/>

</xml_diff>

<commit_message>
Updated to fix exploration failure and minor changes in Config3 test data
</commit_message>
<xml_diff>
--- a/Resources/Configuration3.xlsx
+++ b/Resources/Configuration3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MugunthRaman\git\EagleAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BFF6CD-09AE-4723-8091-36AB903D47FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56EB8831-0309-4075-9EC0-90DE22C5180D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3883F32-F6B7-4344-89C2-CDCBDBE1FA77}"/>
   </bookViews>
@@ -684,9 +684,6 @@
     <t>&lt;Exploration Name to be created&gt;,&lt;entity to be selected&gt;,&lt;search text for creating Exploration&gt;,&lt;Item 1 to be removed&gt;, &lt;Item 2 to be removed&gt;,&lt;Item 3 to be removed&gt;</t>
   </si>
   <si>
-    <t>Remove Item Exploration,RNA,asb,AL160411.1,AC060814.4,AL022100.1</t>
-  </si>
-  <si>
     <t>Sort_Column_Exploration</t>
   </si>
   <si>
@@ -771,9 +768,6 @@
     <t>&lt;Comparison Name to be created&gt;, &lt;Control Set Name&gt;, &lt;Case set Name&gt;, &lt;entity to be selected&gt;, &lt;search text for creating Comparison control&gt;, &lt;search text for creating Comparison case&gt;</t>
   </si>
   <si>
-    <t>Comparison Control and Case 1, Control Set, Case Set, Disease, kera,buy</t>
-  </si>
-  <si>
     <t>createComparisonWithControlandCaseRunComparison</t>
   </si>
   <si>
@@ -783,9 +777,6 @@
     <t>Create a comparison with a control card and a case card and also run comparison</t>
   </si>
   <si>
-    <t>Comparison Control and Case 2, Control Set, Case Set,Disease, kera,buy</t>
-  </si>
-  <si>
     <t>updateComparisonWithCaseCard</t>
   </si>
   <si>
@@ -990,9 +981,6 @@
     <t>&lt;Comparison Name to be selected&gt;,&lt;Control Set Name&gt;,&lt;entity to be selected&gt;, &lt;search text for creating Comparison control&gt;,&lt;1st item to be removed&gt;,&lt;2nd item to be removed&gt;,&lt;3rd item to be removed&gt;</t>
   </si>
   <si>
-    <t>Remove Item Comparison,Control Set ,Gene,asph,72112780,20981360,147670524</t>
-  </si>
-  <si>
     <t>ChangeControlAndCase</t>
   </si>
   <si>
@@ -1138,6 +1126,18 @@
   </si>
   <si>
     <t>DComparison2Card, Control Card,Case Card ,Disease, kera,worm</t>
+  </si>
+  <si>
+    <t>Remove Item Comparison,Control Set ,Gene,asph,61714649,23827690,12022680</t>
+  </si>
+  <si>
+    <t>Remove Item Exploration,RNA,asb,ASB16,ASB15,ASB14</t>
+  </si>
+  <si>
+    <t>Comparison Control and Case 2, Control Set, Case Set,Disease, kera,bur</t>
+  </si>
+  <si>
+    <t>Comparison Control and Case 1, Control Set, Case Set, Disease, kera,bur</t>
   </si>
 </sst>
 </file>
@@ -1892,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6CDC57-9314-4DDE-912B-780BF34D9001}">
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="C49" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2108,7 +2108,7 @@
         <v>66</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G11" s="32"/>
       <c r="H11" s="10"/>
@@ -2203,7 +2203,7 @@
         <v>90</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="G16" s="32"/>
       <c r="H16" s="10"/>
@@ -2245,7 +2245,7 @@
       </c>
       <c r="G18" s="32"/>
       <c r="H18" s="28" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2262,7 +2262,7 @@
         <v>103</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="G19" s="32"/>
       <c r="H19" s="10"/>
@@ -2380,7 +2380,7 @@
       </c>
       <c r="G25" s="32"/>
       <c r="H25" s="28" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="G26" s="33"/>
       <c r="H26" s="28" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2477,7 +2477,7 @@
         <v>149</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="G30" s="34"/>
       <c r="H30" s="10"/>
@@ -2610,7 +2610,7 @@
         <v>182</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="G37" s="34"/>
       <c r="H37" s="10"/>
@@ -2743,72 +2743,72 @@
         <v>215</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>216</v>
+        <v>365</v>
       </c>
       <c r="G44" s="34"/>
       <c r="H44" s="28" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="E45" s="6" t="s">
         <v>220</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>221</v>
       </c>
       <c r="G45" s="34"/>
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="E46" s="6" t="s">
         <v>225</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>226</v>
       </c>
       <c r="G46" s="34"/>
       <c r="H46" s="28" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="B47" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="B47" s="23" t="s">
+      <c r="C47" s="23" t="s">
         <v>228</v>
       </c>
-      <c r="C47" s="23" t="s">
+      <c r="D47" s="23" t="s">
         <v>229</v>
       </c>
-      <c r="D47" s="23" t="s">
+      <c r="E47" s="25" t="s">
         <v>230</v>
-      </c>
-      <c r="E47" s="25" t="s">
-        <v>231</v>
       </c>
       <c r="G47" s="35"/>
       <c r="H47" s="28" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2834,437 +2834,437 @@
     </row>
     <row r="49" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="E49" s="6" t="s">
         <v>235</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>236</v>
       </c>
       <c r="G49" s="34"/>
       <c r="H49" s="10"/>
     </row>
     <row r="50" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="E50" s="6" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="G50" s="34"/>
       <c r="H50" s="10"/>
     </row>
     <row r="51" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>244</v>
-      </c>
       <c r="E51" s="6" t="s">
-        <v>245</v>
+        <v>367</v>
       </c>
       <c r="G51" s="34"/>
       <c r="H51" s="10"/>
     </row>
     <row r="52" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>248</v>
-      </c>
       <c r="D52" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>249</v>
+        <v>366</v>
       </c>
       <c r="G52" s="34"/>
       <c r="H52" s="10"/>
     </row>
     <row r="53" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>253</v>
-      </c>
       <c r="E53" s="6" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="G53" s="34"/>
       <c r="H53" s="10"/>
     </row>
     <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="E54" s="6" t="s">
         <v>255</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>258</v>
       </c>
       <c r="G54" s="34"/>
       <c r="H54" s="10"/>
     </row>
     <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="E55" s="6" t="s">
         <v>260</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>263</v>
       </c>
       <c r="G55" s="34"/>
       <c r="H55" s="10"/>
     </row>
     <row r="56" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E56" s="6" t="s">
         <v>264</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>267</v>
       </c>
       <c r="G56" s="34"/>
       <c r="H56" s="10"/>
     </row>
     <row r="57" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>271</v>
-      </c>
       <c r="E57" s="6" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="G57" s="34"/>
       <c r="H57" s="10"/>
     </row>
     <row r="58" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="E58" s="6" t="s">
         <v>273</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>276</v>
       </c>
       <c r="G58" s="34"/>
       <c r="H58" s="10"/>
     </row>
     <row r="59" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="E59" s="6" t="s">
         <v>278</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>281</v>
       </c>
       <c r="G59" s="34"/>
       <c r="H59" s="10"/>
     </row>
     <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>90</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="G60" s="34"/>
       <c r="H60" s="10"/>
     </row>
     <row r="61" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="E61" s="6" t="s">
         <v>286</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>289</v>
       </c>
       <c r="G61" s="34"/>
       <c r="H61" s="10"/>
     </row>
     <row r="62" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E62" s="6" t="s">
         <v>290</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>293</v>
       </c>
       <c r="G62" s="34"/>
       <c r="H62" s="10"/>
     </row>
     <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="E63" s="6" t="s">
         <v>295</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>298</v>
       </c>
       <c r="G63" s="34"/>
       <c r="H63" s="10"/>
     </row>
     <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="E64" s="6" t="s">
         <v>300</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>303</v>
       </c>
       <c r="G64" s="34"/>
       <c r="H64" s="10"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="E65" s="6" t="s">
         <v>305</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>308</v>
       </c>
       <c r="G65" s="34"/>
       <c r="H65" s="10"/>
     </row>
     <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="E66" s="6" t="s">
         <v>310</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>313</v>
       </c>
       <c r="G66" s="34"/>
       <c r="H66" s="10"/>
     </row>
     <row r="67" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="E67" s="6" t="s">
-        <v>318</v>
+        <v>364</v>
       </c>
       <c r="G67" s="34"/>
       <c r="H67" s="10"/>
     </row>
     <row r="68" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E68" s="6" t="s">
         <v>319</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>323</v>
       </c>
       <c r="G68" s="34"/>
       <c r="H68" s="10"/>
     </row>
     <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E69" s="6" t="s">
         <v>324</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>328</v>
       </c>
       <c r="G69" s="34"/>
       <c r="H69" s="10"/>
     </row>
     <row r="70" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="G70" s="34"/>
       <c r="H70" s="10"/>
     </row>
     <row r="71" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C71" s="23" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="D71" s="23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="G71" s="34"/>
       <c r="H71" s="10"/>
@@ -3288,93 +3288,93 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="G73" s="30"/>
       <c r="H73" s="10"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="G74" s="30"/>
       <c r="H74" s="10"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G75" s="30"/>
       <c r="H75" s="10"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="G76" s="30"/>
       <c r="H76" s="10"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="G77" s="30"/>
       <c r="H77" s="10"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="G78" s="30"/>
       <c r="H78" s="10"/>
     </row>
     <row r="79" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="26" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B79" s="23" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C79" s="23"/>
       <c r="D79" s="23"/>
       <c r="E79" s="25" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="G79" s="37"/>
       <c r="H79" s="10"/>

</xml_diff>

<commit_message>
Updated for the fixes after complete run on 24th Dec
The following are implemented:
1) move to top for checking the expand name of card
2) Add a screenshot to add to grid not selectable
</commit_message>
<xml_diff>
--- a/Resources/Configuration3.xlsx
+++ b/Resources/Configuration3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MugunthRaman\git\EagleAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C1435E-002F-403F-A6D3-91E6105ADCEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9D0DCE-859E-465E-8FB2-5DEAA41504D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3883F32-F6B7-4344-89C2-CDCBDBE1FA77}"/>
   </bookViews>
@@ -1895,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6CDC57-9314-4DDE-912B-780BF34D9001}">
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C71" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72:E79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Made fixes in Sets, Exploration and Comparison.
1) Fixes for Sort Column
2) Fixes for Remove items (Change in Test Data in Configuration3 file)
</commit_message>
<xml_diff>
--- a/Resources/Configuration3.xlsx
+++ b/Resources/Configuration3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MugunthRaman\git\EagleAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613BB790-70CD-4B32-AD43-1A85858D9313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49784F6D-ABF5-4D93-92CD-48FB8C9AE8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3883F32-F6B7-4344-89C2-CDCBDBE1FA77}"/>
   </bookViews>
@@ -1182,13 +1182,14 @@
     <t>Analysis-2, Test Description for Analysis Check,Galleon</t>
   </si>
   <si>
-    <t>Remove Item Set, Disease, sulf, MONDO_0018640,EFO_0008283, EFO_0008422</t>
-  </si>
-  <si>
-    <t>Remove Item Exploration,RNA,asb,AC018521.6,ACLY,HOXB-AS3</t>
-  </si>
-  <si>
-    <t>Remove Item Comparison,Control Set ,Gene,asph,611296,600582,300297</t>
+    <t>Remove Item Comparison,Control Set ,Gene,asph,
+6333612,236131800,101161596</t>
+  </si>
+  <si>
+    <t>Remove Item Set, Disease, sulf,EFO_0000689,EFO_1000532, EFO_0008403</t>
+  </si>
+  <si>
+    <t>Remove Item Exploration,RNA,asb,AC004980.3,AC007652.1,AC027644.3</t>
   </si>
 </sst>
 </file>
@@ -1956,7 +1957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6CDC57-9314-4DDE-912B-780BF34D9001}">
   <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
@@ -2356,7 +2357,7 @@
         <v>95</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="G21" s="35"/>
       <c r="H21" s="26" t="s">
@@ -2858,7 +2859,7 @@
         <v>207</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G47" s="37"/>
       <c r="H47" s="26" t="s">
@@ -3303,7 +3304,7 @@
         <v>304</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G70" s="37"/>
       <c r="H70" s="10"/>

</xml_diff>

<commit_message>
Made changes in configuration3 file
</commit_message>
<xml_diff>
--- a/Resources/Configuration3.xlsx
+++ b/Resources/Configuration3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MugunthRaman\git\EagleAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B8DB83-35E4-4E22-AAB8-FDF30D5FE194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032F5479-098B-4952-8D65-3B903B031B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3883F32-F6B7-4344-89C2-CDCBDBE1FA77}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="406">
   <si>
     <t>Skin Care, This is to analyse about the skin</t>
   </si>
@@ -1164,9 +1164,6 @@
     <t>&lt;AnalysisName&gt;, &lt;AnalysisDescription&gt;, &lt;studyName&gt;</t>
   </si>
   <si>
-    <t>Analysis-1,Analysis Description,Galleon</t>
-  </si>
-  <si>
     <t>Analysis</t>
   </si>
   <si>
@@ -1177,9 +1174,6 @@
   </si>
   <si>
     <t>Create an analysis after doing all the mandatory field check</t>
-  </si>
-  <si>
-    <t>Analysis-2, Test Description for Analysis Check,Galleon</t>
   </si>
   <si>
     <t>Remove Item Comparison,Control Set ,Gene,asph,
@@ -1190,6 +1184,75 @@
   </si>
   <si>
     <t>Remove Item Exploration,RNA,asb,AC004980.3,AC007652.1,AC027644.3</t>
+  </si>
+  <si>
+    <t>Analysis-1,Analysis Description,Eagle Study A</t>
+  </si>
+  <si>
+    <t>Analysis-2, Test Description for Analysis Check,Eagle Study A</t>
+  </si>
+  <si>
+    <t>AnalysisNameAndDescEditInList</t>
+  </si>
+  <si>
+    <t>AnalysisNameAndDescEditInList_Test</t>
+  </si>
+  <si>
+    <t>Create an Analysis and Edit the name and description from the list view</t>
+  </si>
+  <si>
+    <t>&lt;AnalysisNameInital&gt;, &lt;AnalysisDescriptionInital&gt;, &lt;StudyName&gt;, &lt;AnalysisName&gt;, &lt;AnalysisDescription&gt;</t>
+  </si>
+  <si>
+    <t>Analysis-3,Analysis Description,Eagle Study A,Name of [Analysis&gt;: is changed, Description of [Analysis&gt;: is changed</t>
+  </si>
+  <si>
+    <t>AnalysisNameAndDescEditInPage</t>
+  </si>
+  <si>
+    <t>AnalysisNameAndDescEditInPage_Test</t>
+  </si>
+  <si>
+    <t>Create an Analysis and Edit the name and description inside the analysis page view</t>
+  </si>
+  <si>
+    <t>Analysis-4,Far far away behind the word mountains far from the countries Vokalia and Consonantia there live the blind texts. Separated they live in Bookmarksgrove right at the coast of the Semantics a large language ocean. A small river named Duden flows by their place and supplies it with the necessary regelialia. It is a paradisematic country in which roasted parts of sentences fly into your mouth. Even the all-powerful Pointing has no control about the blind texts it is an almost unorthographic life One day however a small line of blind text by the name of Lorem Ipsum decided to leave for the far,Eagle Study A,Name of ()@#$Analysis{}: is changed, Description small, Description of ()@#$Analysis{}: is changed</t>
+  </si>
+  <si>
+    <t>CreateAndDeleteAnalysis</t>
+  </si>
+  <si>
+    <t>CreateAndDeleteAnalysis_Test</t>
+  </si>
+  <si>
+    <t>Create an Analysis and Delete the same</t>
+  </si>
+  <si>
+    <t>Analysis-5,Analysis Description,Eagle Study A</t>
+  </si>
+  <si>
+    <t>VerifyNumericalValueAnalysis</t>
+  </si>
+  <si>
+    <t>VerifyNumericalValueAnalysis_Test</t>
+  </si>
+  <si>
+    <t>Create an Analysis and select a Numerical feature and verify the labels</t>
+  </si>
+  <si>
+    <t>&lt;AnalysisName&gt;, &lt;AnalysisDescription&gt;, &lt;studyName&gt;, &lt;Entity Name&gt;, &lt;Feature Name&gt;</t>
+  </si>
+  <si>
+    <t>Numerical Value Analysis, Numerical Value Analysis, Eagle Study A,Subject,body_mass_index</t>
+  </si>
+  <si>
+    <t>VerifyCategoticalValueAnalysis</t>
+  </si>
+  <si>
+    <t>VerifyCategoticalValueAnalysis_Test</t>
+  </si>
+  <si>
+    <t>Categorical Value Analysis, Categorical Value Analysis,Eagle Study A,Subject,disease</t>
   </si>
 </sst>
 </file>
@@ -1645,8 +1708,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9F58C19D-99E7-4933-ADBF-D8A1FC7A4A8F}" name="Table2" displayName="Table2" ref="A1:E89" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E89" xr:uid="{9F58C19D-99E7-4933-ADBF-D8A1FC7A4A8F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9F58C19D-99E7-4933-ADBF-D8A1FC7A4A8F}" name="Table2" displayName="Table2" ref="A1:E90" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E90" xr:uid="{9F58C19D-99E7-4933-ADBF-D8A1FC7A4A8F}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{E4EE8482-C9A5-4BE2-A04A-30789F6C4A9B}" name="Test Case#" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{6C42973B-7CD5-4DF3-A4E4-2D87D248B024}" name="FunctionName" dataDxfId="3"/>
@@ -1955,10 +2018,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6CDC57-9314-4DDE-912B-780BF34D9001}">
-  <dimension ref="A1:H89"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="C28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H86" sqref="H29:H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2357,7 +2420,7 @@
         <v>95</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G21" s="35"/>
       <c r="H21" s="26" t="s">
@@ -2859,7 +2922,7 @@
         <v>207</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G47" s="37"/>
       <c r="H47" s="26" t="s">
@@ -3304,7 +3367,7 @@
         <v>304</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G70" s="37"/>
       <c r="H70" s="10"/>
@@ -3509,81 +3572,149 @@
         <v>375</v>
       </c>
       <c r="E83" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="G83" s="31" t="s">
         <v>376</v>
-      </c>
-      <c r="G83" s="31" t="s">
-        <v>377</v>
       </c>
       <c r="H83" s="10"/>
     </row>
     <row r="84" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>380</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>375</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="G84" s="32"/>
       <c r="H84" s="10"/>
     </row>
-    <row r="85" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="8"/>
-      <c r="E85" s="6"/>
+    <row r="85" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A85" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>389</v>
+      </c>
       <c r="G85" s="32"/>
       <c r="H85" s="10"/>
     </row>
-    <row r="86" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="8"/>
-      <c r="E86" s="6"/>
+    <row r="86" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="A86" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>393</v>
+      </c>
       <c r="G86" s="32"/>
       <c r="H86" s="10"/>
     </row>
-    <row r="87" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="8"/>
-      <c r="E87" s="6"/>
+    <row r="87" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>397</v>
+      </c>
       <c r="G87" s="32"/>
       <c r="H87" s="10"/>
     </row>
-    <row r="88" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="24"/>
-      <c r="B88" s="21"/>
-      <c r="C88" s="21"/>
-      <c r="D88" s="21"/>
-      <c r="E88" s="23"/>
-      <c r="G88" s="33"/>
+    <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="G88" s="32"/>
       <c r="H88" s="10"/>
     </row>
-    <row r="89" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="14" t="s">
+    <row r="89" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="G89" s="33"/>
+      <c r="H89" s="10"/>
+    </row>
+    <row r="90" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D89" s="15" t="s">
+      <c r="D90" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E89" s="3"/>
-      <c r="G89" s="16" t="s">
+      <c r="E90" s="3"/>
+      <c r="G90" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H89" s="10"/>
+      <c r="H90" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="G83:G88"/>
+    <mergeCell ref="G83:G89"/>
     <mergeCell ref="G3:G11"/>
     <mergeCell ref="G12:G29"/>
     <mergeCell ref="G30:G50"/>

</xml_diff>

<commit_message>
Updated with minor changes in Analysis for the plot headers verification and also changed configuration 3
</commit_message>
<xml_diff>
--- a/Resources/Configuration3.xlsx
+++ b/Resources/Configuration3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MugunthRaman\git\EagleAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{882847EC-F7F4-4ED4-9D26-42522F68D490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{882847EC-F7F4-4ED4-9D26-42522F68D490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86F79544-9690-4607-97A5-4999AA643028}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3883F32-F6B7-4344-89C2-CDCBDBE1FA77}"/>
   </bookViews>
@@ -682,7 +682,7 @@
     <t>&lt;Exploration Name to be created&gt;,&lt;entity to be selected&gt;,&lt;search text for creating Exploration&gt;,&lt;Item 1 to be removed&gt;, &lt;Item 2 to be removed&gt;,&lt;Item 3 to be removed&gt;</t>
   </si>
   <si>
-    <t>Remove Item Exploration,RNA,asb,ASB12,ASB16-AS1,ASB6</t>
+    <t>Remove Item Exploration,RNA,asb,AC026316.2,AC083906.1,ADCY5</t>
   </si>
   <si>
     <t>Sort_Column_Exploration</t>
@@ -1240,7 +1240,7 @@
     <t>Verify if the expand and different views of Graph canvas are working fine</t>
   </si>
   <si>
-    <t>Resizing Graph Canvas Analysis,Resizing Graph Canvas Analysis,2</t>
+    <t>Resizing Graph Canvas Analysis,Resizing Graph Canvas Analysis,1</t>
   </si>
   <si>
     <t>EntitiesAndFeatureSelectionVerificationInGraph</t>
@@ -1279,7 +1279,7 @@
     <t>Create and Verify different plots with one categorical value</t>
   </si>
   <si>
-    <t>CategoricalPlot1,CategoricalPlot1,2,2,0</t>
+    <t>CategoricalPlot1,CategoricalPlot1,1,2,0</t>
   </si>
   <si>
     <t>PlotWithOneCategoricalandOneNumericalFeature</t>
@@ -1291,7 +1291,7 @@
     <t>Create and Verify different plots with one numeric and one categorical value</t>
   </si>
   <si>
-    <t>1Categorical1NumericalPlot,1Categorical1NumericalPlot,3,2,2</t>
+    <t>1Categorical1NumericalPlot,1Categorical1NumericalPlot,1,2,2</t>
   </si>
   <si>
     <t>PlotWithTwoNumericalFeature</t>
@@ -1315,7 +1315,7 @@
     <t>Create and Verify different plots with two categoric values</t>
   </si>
   <si>
-    <t>2CategoricalPlots,2CategoricalPlots,2,3,0</t>
+    <t>2CategoricalPlots,2CategoricalPlots,1,3,0</t>
   </si>
   <si>
     <t>PlotWithTwoNumericalandOneCategoricalFeatures</t>
@@ -1327,7 +1327,7 @@
     <t>Create and Verify different plots with two numeric and one categoric values</t>
   </si>
   <si>
-    <t>2Numerical1CategoricalPlots,2Numerical1CategoricalPlots,2,2,3</t>
+    <t>2Numerical1CategoricalPlots,2Numerical1CategoricalPlots,1,2,3</t>
   </si>
   <si>
     <t>PlotWithThreeNumericalFeatures</t>
@@ -2198,8 +2198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6CDC57-9314-4DDE-912B-780BF34D9001}">
   <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B65" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="B92" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4082,21 +4082,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005EDAA1EB1D58B449A665C8960057699D" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="70f6f9e5c7980eb9729804970d16a34b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="db720d58-4227-411f-bcee-c8e33b64d7b1" xmlns:ns3="63945a94-eccf-4e51-b06e-13c7875d9720" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="10a4f86fcee4fdd6d37add7357595ef5" ns2:_="" ns3:_="">
     <xsd:import namespace="db720d58-4227-411f-bcee-c8e33b64d7b1"/>
@@ -4313,14 +4298,29 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C28275C4-6DA4-4542-8FDD-81BE0D18CB72}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7725FD0A-4BC1-400F-86E8-AEC58AFD64C5}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB5D6A75-DF1A-4E66-A542-95A7A294D24A}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C28275C4-6DA4-4542-8FDD-81BE0D18CB72}"/>
 </file>
</xml_diff>